<commit_message>
added stats for alpha diversity in P,N and F
</commit_message>
<xml_diff>
--- a/metadata_unified.xlsx
+++ b/metadata_unified.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elsa/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elsa/Desktop/THESIS/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21A5B30-695C-0C44-A3EF-455DC2099534}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D2167A-ED5D-6E45-B0FB-790FE3E6D591}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6140" yWindow="520" windowWidth="22660" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22660" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -901,12 +901,6 @@
     <t>Tania_serialis</t>
   </si>
   <si>
-    <t>toxoplasma_gondii</t>
-  </si>
-  <si>
-    <t>trichincella_spp</t>
-  </si>
-  <si>
     <t>Pack</t>
   </si>
   <si>
@@ -1004,6 +998,12 @@
   </si>
   <si>
     <t>P10</t>
+  </si>
+  <si>
+    <t>sero_toxoplasma_gondii</t>
+  </si>
+  <si>
+    <t>sero_trichincella_spp</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1039,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1049,6 +1049,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1065,7 +1095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1076,6 +1106,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1417,7 +1457,7 @@
   <dimension ref="A1:AE87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1471,16 +1511,16 @@
         <v>144</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>295</v>
-      </c>
       <c r="N1" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>2</v>
@@ -1541,35 +1581,35 @@
       <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F2" t="s">
-        <v>280</v>
-      </c>
-      <c r="G2" t="s">
-        <v>280</v>
-      </c>
-      <c r="H2" t="s">
-        <v>280</v>
-      </c>
-      <c r="I2" t="s">
-        <v>280</v>
-      </c>
-      <c r="J2" t="s">
-        <v>280</v>
-      </c>
-      <c r="K2" t="s">
-        <v>280</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="F2" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>280</v>
       </c>
       <c r="M2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O2" t="s">
         <v>21</v>
@@ -1633,35 +1673,35 @@
       <c r="C3" t="s">
         <v>267</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F3" t="s">
-        <v>280</v>
-      </c>
-      <c r="G3" t="s">
-        <v>280</v>
-      </c>
-      <c r="H3" t="s">
-        <v>280</v>
-      </c>
-      <c r="I3" t="s">
-        <v>280</v>
-      </c>
-      <c r="J3" t="s">
-        <v>280</v>
-      </c>
-      <c r="K3" t="s">
-        <v>280</v>
-      </c>
-      <c r="L3" t="s">
-        <v>280</v>
+      <c r="F3" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="M3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N3">
         <v>3</v>
@@ -1725,35 +1765,35 @@
       <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F4" t="s">
-        <v>280</v>
-      </c>
-      <c r="G4" t="s">
-        <v>280</v>
-      </c>
-      <c r="H4" t="s">
-        <v>280</v>
-      </c>
-      <c r="I4" t="s">
-        <v>280</v>
-      </c>
-      <c r="J4" t="s">
-        <v>280</v>
-      </c>
-      <c r="K4" t="s">
-        <v>280</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="F4" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>280</v>
       </c>
       <c r="M4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O4" t="s">
         <v>21</v>
@@ -1814,35 +1854,35 @@
       <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="8" t="s">
         <v>148</v>
       </c>
       <c r="M5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="O5" t="s">
         <v>21</v>
@@ -1906,35 +1946,35 @@
       <c r="C6" t="s">
         <v>243</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="G6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="G6" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="J6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L6" t="s">
-        <v>280</v>
+      <c r="J6" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="M6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="N6">
         <v>4</v>
@@ -2001,35 +2041,35 @@
       <c r="C7" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="H7" s="5" t="s">
+      <c r="F7" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>280</v>
+      <c r="I7" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="N7" s="5">
         <v>3</v>
@@ -2096,35 +2136,35 @@
       <c r="C8" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>280</v>
+      <c r="F8" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N8" s="6">
         <v>4</v>
@@ -2191,35 +2231,35 @@
       <c r="C9" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>280</v>
+      <c r="G9" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="N9" s="6">
         <v>4</v>
@@ -2284,35 +2324,35 @@
         <v>45</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L10" s="6" t="s">
+      <c r="F10" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L10" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" t="s">
@@ -2375,35 +2415,35 @@
         <v>47</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L11" s="6" t="s">
+      <c r="F11" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L11" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="N11" s="6"/>
       <c r="O11" t="s">
@@ -2466,35 +2506,35 @@
         <v>49</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I12" s="6" t="s">
+      <c r="F12" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="J12" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L12" s="6" t="s">
+      <c r="J12" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L12" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" t="s">
@@ -2559,35 +2599,35 @@
       <c r="C13" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>280</v>
+      <c r="F13" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="N13" s="5">
         <v>3</v>
@@ -2652,35 +2692,35 @@
         <v>53</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L14" s="6" t="s">
+      <c r="F14" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L14" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" t="s">
@@ -2745,35 +2785,35 @@
       <c r="C15" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>280</v>
+      <c r="G15" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="N15" s="6">
         <v>3</v>
@@ -2840,35 +2880,35 @@
       <c r="C16" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>280</v>
+      <c r="G16" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="N16" s="6">
         <v>4</v>
@@ -2935,35 +2975,35 @@
       <c r="C17" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I17" s="6" t="s">
+      <c r="H17" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I17" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="K17" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>280</v>
+      <c r="K17" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="N17" s="6">
         <v>4</v>
@@ -3030,35 +3070,35 @@
       <c r="C18" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>280</v>
+      <c r="F18" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="N18" s="6">
         <v>2</v>
@@ -3125,35 +3165,35 @@
       <c r="C19" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>280</v>
+      <c r="F19" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="N19" s="6">
         <v>3</v>
@@ -3218,35 +3258,35 @@
         <v>65</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="J20" s="6" t="s">
+      <c r="J20" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="K20" s="6" t="s">
+      <c r="K20" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="L20" s="6" t="s">
+      <c r="L20" s="13" t="s">
         <v>148</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="N20" s="6"/>
       <c r="O20" t="s">
@@ -3311,35 +3351,35 @@
       <c r="C21" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>280</v>
+      <c r="F21" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="N21" s="6">
         <v>4</v>
@@ -3404,35 +3444,35 @@
         <v>69</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F22" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L22" s="6" t="s">
+      <c r="F22" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L22" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="N22" s="6"/>
       <c r="O22" t="s">
@@ -3497,35 +3537,35 @@
       <c r="C23" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>280</v>
+      <c r="F23" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="N23" s="5">
         <v>3</v>
@@ -3592,35 +3632,35 @@
       <c r="C24" t="s">
         <v>259</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>280</v>
+      <c r="G24" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="N24" s="6">
         <v>2</v>
@@ -3684,35 +3724,35 @@
       <c r="B25" t="s">
         <v>75</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L25" s="6" t="s">
+      <c r="F25" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L25" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="N25" s="6"/>
       <c r="O25" t="s">
@@ -3774,35 +3814,35 @@
       <c r="B26" t="s">
         <v>77</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F26" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L26" s="6" t="s">
+      <c r="F26" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L26" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="N26" s="6"/>
       <c r="O26" t="s">
@@ -3864,35 +3904,35 @@
       <c r="B27" t="s">
         <v>79</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L27" s="6" t="s">
+      <c r="F27" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L27" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N27" s="6"/>
       <c r="O27" t="s">
@@ -3954,35 +3994,35 @@
       <c r="B28" t="s">
         <v>81</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K28" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="L28" t="s">
+      <c r="L28" s="8" t="s">
         <v>148</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="N28" s="6"/>
       <c r="O28" t="s">
@@ -4047,35 +4087,35 @@
       <c r="C29" t="s">
         <v>240</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F29" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>280</v>
+      <c r="F29" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="L29" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N29" s="6">
         <v>4</v>
@@ -4142,35 +4182,35 @@
       <c r="C30" t="s">
         <v>272</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L30" s="6" t="s">
-        <v>280</v>
+      <c r="F30" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M30" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="N30" s="6">
         <v>3</v>
@@ -4237,35 +4277,35 @@
       <c r="C31" t="s">
         <v>258</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G31" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I31" s="6" t="s">
+      <c r="H31" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I31" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="J31" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L31" s="6" t="s">
-        <v>280</v>
+      <c r="J31" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="N31" s="6">
         <v>4</v>
@@ -4329,35 +4369,35 @@
       <c r="B32" t="s">
         <v>89</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L32" s="6" t="s">
+      <c r="F32" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K32" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L32" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N32" s="6"/>
       <c r="O32" t="s">
@@ -4419,35 +4459,35 @@
       <c r="B33" t="s">
         <v>91</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L33" s="6" t="s">
+      <c r="F33" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L33" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="N33" s="6"/>
       <c r="O33" t="s">
@@ -4512,35 +4552,35 @@
       <c r="C34" t="s">
         <v>270</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F34" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I34" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L34" s="6" t="s">
-        <v>280</v>
+      <c r="F34" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L34" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="N34" s="6">
         <v>3</v>
@@ -4604,35 +4644,35 @@
       <c r="B35" t="s">
         <v>95</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J35" s="6" t="s">
+      <c r="F35" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J35" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="K35" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L35" s="6" t="s">
+      <c r="K35" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L35" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="N35" s="6"/>
       <c r="O35" t="s">
@@ -4694,35 +4734,35 @@
       <c r="B36" t="s">
         <v>97</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J36" s="6" t="s">
+      <c r="F36" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J36" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="K36" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L36" s="6" t="s">
+      <c r="K36" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L36" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="N36" s="6"/>
       <c r="O36" t="s">
@@ -4784,35 +4824,35 @@
       <c r="B37" t="s">
         <v>99</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F37" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K37" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L37" s="6" t="s">
+      <c r="F37" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L37" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="N37" s="6"/>
       <c r="O37" t="s">
@@ -4877,35 +4917,35 @@
       <c r="C38" t="s">
         <v>266</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F38" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K38" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L38" s="6" t="s">
-        <v>280</v>
+      <c r="F38" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="L38" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="N38" s="6">
         <v>4</v>
@@ -4969,35 +5009,35 @@
       <c r="B39" t="s">
         <v>103</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F39" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K39" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L39" s="6" t="s">
+      <c r="F39" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K39" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L39" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="N39" s="6"/>
       <c r="O39" t="s">
@@ -5062,35 +5102,35 @@
       <c r="C40" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F40" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I40" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J40" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K40" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L40" s="6" t="s">
-        <v>280</v>
+      <c r="F40" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K40" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="L40" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N40" s="6">
         <v>4</v>
@@ -5157,35 +5197,35 @@
       <c r="C41" t="s">
         <v>271</v>
       </c>
-      <c r="D41" t="s">
-        <v>302</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="D41" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K41" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L41" s="6" t="s">
-        <v>280</v>
+      <c r="F41" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L41" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="N41" s="6">
         <v>3</v>
@@ -5249,35 +5289,35 @@
       <c r="B42" t="s">
         <v>109</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I42" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K42" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L42" s="6" t="s">
+      <c r="F42" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J42" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K42" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L42" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M42" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="N42" s="6"/>
       <c r="O42" t="s">
@@ -5342,35 +5382,35 @@
       <c r="C43" t="s">
         <v>273</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F43" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="G43" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="H43" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K43" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L43" s="6" t="s">
-        <v>280</v>
+      <c r="H43" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K43" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="L43" s="12" t="s">
+        <v>148</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="N43" s="6">
         <v>3</v>
@@ -5434,35 +5474,35 @@
       <c r="B44" t="s">
         <v>113</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F44" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K44" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L44" s="6" t="s">
+      <c r="F44" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J44" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K44" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L44" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M44" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="N44" s="6"/>
       <c r="O44" t="s">
@@ -5527,35 +5567,35 @@
       <c r="C45" t="s">
         <v>269</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F45" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I45" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L45" s="6" t="s">
-        <v>280</v>
+      <c r="F45" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I45" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J45" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K45" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="N45" s="6">
         <v>3</v>
@@ -5622,35 +5662,35 @@
       <c r="C46" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F46" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I46" s="6" t="s">
+      <c r="F46" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H46" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I46" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="J46" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K46" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L46" s="6" t="s">
-        <v>280</v>
+      <c r="J46" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K46" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="L46" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="N46" s="6"/>
       <c r="O46" t="s">
@@ -5712,35 +5752,35 @@
       <c r="B47" t="s">
         <v>119</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F47" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K47" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L47" s="6" t="s">
+      <c r="F47" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J47" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K47" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L47" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="N47" s="6"/>
       <c r="O47" t="s">
@@ -5802,35 +5842,35 @@
       <c r="B48" t="s">
         <v>121</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F48" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J48" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K48" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L48" s="6" t="s">
+      <c r="F48" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J48" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K48" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L48" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M48" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="N48" s="6"/>
       <c r="O48" t="s">
@@ -5895,35 +5935,35 @@
       <c r="C49" t="s">
         <v>257</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F49" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I49" s="6" t="s">
+      <c r="F49" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H49" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I49" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="J49" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K49" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L49" s="6" t="s">
-        <v>280</v>
+      <c r="J49" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K49" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="L49" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="N49" s="6">
         <v>2</v>
@@ -5987,35 +6027,35 @@
       <c r="B50" t="s">
         <v>125</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F50" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I50" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K50" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L50" s="6" t="s">
+      <c r="F50" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K50" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L50" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M50" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="N50" s="6"/>
       <c r="O50" t="s">
@@ -6077,35 +6117,35 @@
       <c r="B51" t="s">
         <v>127</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F51" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J51" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K51" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L51" s="6" t="s">
+      <c r="F51" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I51" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J51" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K51" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L51" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="N51" s="6"/>
       <c r="O51" t="s">
@@ -6170,35 +6210,35 @@
       <c r="C52" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="G52" t="s">
-        <v>280</v>
-      </c>
-      <c r="H52" t="s">
-        <v>280</v>
-      </c>
-      <c r="I52" t="s">
-        <v>280</v>
-      </c>
-      <c r="J52" t="s">
-        <v>280</v>
-      </c>
-      <c r="K52" t="s">
-        <v>280</v>
-      </c>
-      <c r="L52" t="s">
-        <v>280</v>
+      <c r="G52" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="I52" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="J52" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="K52" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="L52" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="M52" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="N52">
         <v>2</v>
@@ -6265,35 +6305,35 @@
       <c r="C53" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="E53" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F53" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H53" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J53" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K53" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L53" s="6" t="s">
-        <v>280</v>
+      <c r="F53" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J53" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K53" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="L53" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M53" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N53" s="6">
         <v>3</v>
@@ -6357,35 +6397,35 @@
       <c r="B54" t="s">
         <v>132</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F54" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I54" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J54" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K54" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L54" s="6" t="s">
+      <c r="F54" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J54" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K54" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L54" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M54" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="N54" s="6"/>
       <c r="O54" t="s">
@@ -6450,35 +6490,35 @@
       <c r="C55" t="s">
         <v>249</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="F55" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="G55" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I55" s="6" t="s">
+      <c r="G55" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H55" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I55" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="J55" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K55" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L55" s="6" t="s">
-        <v>280</v>
+      <c r="J55" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K55" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="L55" s="12" t="s">
+        <v>281</v>
       </c>
       <c r="M55" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="N55" s="6">
         <v>4</v>
@@ -6542,35 +6582,35 @@
       <c r="B56" t="s">
         <v>136</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="F56" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H56" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I56" s="6" t="s">
+      <c r="F56" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I56" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="J56" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K56" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L56" s="6" t="s">
+      <c r="J56" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K56" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L56" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="N56" s="6"/>
       <c r="O56" t="s">
@@ -6632,35 +6672,35 @@
       <c r="B57" t="s">
         <v>138</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F57" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I57" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J57" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K57" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L57" s="6" t="s">
+      <c r="F57" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J57" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K57" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L57" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M57" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="N57" s="6"/>
       <c r="O57" t="s">
@@ -6722,35 +6762,35 @@
       <c r="B58" t="s">
         <v>140</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F58" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I58" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="J58" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="K58" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="L58" s="6" t="s">
+      <c r="F58" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="J58" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="K58" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="L58" s="13" t="s">
         <v>280</v>
       </c>
       <c r="M58" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="N58" s="6"/>
       <c r="O58" t="s">
@@ -6815,35 +6855,35 @@
       <c r="C59" t="s">
         <v>239</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F59" t="s">
-        <v>280</v>
-      </c>
-      <c r="G59" t="s">
-        <v>280</v>
-      </c>
-      <c r="H59" t="s">
-        <v>280</v>
-      </c>
-      <c r="I59" t="s">
-        <v>280</v>
-      </c>
-      <c r="J59" t="s">
-        <v>280</v>
-      </c>
-      <c r="K59" t="s">
-        <v>280</v>
-      </c>
-      <c r="L59" t="s">
-        <v>280</v>
+      <c r="F59" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="I59" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="J59" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="K59" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="L59" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="M59" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="N59">
         <v>3</v>
@@ -6932,7 +6972,7 @@
         <v>280</v>
       </c>
       <c r="M61" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O61" t="s">
         <v>21</v>
@@ -6985,7 +7025,7 @@
         <v>280</v>
       </c>
       <c r="M62" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O62" t="s">
         <v>21</v>
@@ -7038,7 +7078,7 @@
         <v>280</v>
       </c>
       <c r="M63" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="O63" t="s">
         <v>21</v>
@@ -7091,7 +7131,7 @@
         <v>280</v>
       </c>
       <c r="M64" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="O64" t="s">
         <v>21</v>
@@ -7144,7 +7184,7 @@
         <v>280</v>
       </c>
       <c r="M65" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="O65" t="s">
         <v>21</v>
@@ -7197,7 +7237,7 @@
         <v>280</v>
       </c>
       <c r="M66" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="O66" t="s">
         <v>21</v>
@@ -7250,7 +7290,7 @@
         <v>280</v>
       </c>
       <c r="M67" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O67" t="s">
         <v>21</v>
@@ -7303,7 +7343,7 @@
         <v>280</v>
       </c>
       <c r="M68" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="O68" t="s">
         <v>21</v>
@@ -7356,7 +7396,7 @@
         <v>280</v>
       </c>
       <c r="M69" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O69" t="s">
         <v>21</v>
@@ -7409,7 +7449,7 @@
         <v>280</v>
       </c>
       <c r="M70" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="O70" t="s">
         <v>21</v>
@@ -7462,7 +7502,7 @@
         <v>280</v>
       </c>
       <c r="M71" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="O71" t="s">
         <v>21</v>
@@ -7518,7 +7558,7 @@
         <v>280</v>
       </c>
       <c r="M72" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="N72">
         <v>4</v>
@@ -7577,7 +7617,7 @@
         <v>280</v>
       </c>
       <c r="M73" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="N73">
         <v>2</v>
@@ -7636,7 +7676,7 @@
         <v>280</v>
       </c>
       <c r="M74" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="N74">
         <v>3</v>
@@ -7695,7 +7735,7 @@
         <v>280</v>
       </c>
       <c r="M75" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="N75">
         <v>2</v>
@@ -7754,7 +7794,7 @@
         <v>280</v>
       </c>
       <c r="M76" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="N76">
         <v>3</v>
@@ -7813,7 +7853,7 @@
         <v>280</v>
       </c>
       <c r="M77" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="N77">
         <v>3</v>
@@ -7872,7 +7912,7 @@
         <v>280</v>
       </c>
       <c r="M78" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="N78">
         <v>2</v>
@@ -7904,7 +7944,7 @@
         <v>271</v>
       </c>
       <c r="D79" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E79" t="s">
         <v>143</v>
@@ -7931,28 +7971,28 @@
         <v>280</v>
       </c>
       <c r="M79" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="N79">
         <v>3</v>
       </c>
       <c r="O79" t="s">
+        <v>301</v>
+      </c>
+      <c r="P79" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q79" t="s">
         <v>303</v>
       </c>
-      <c r="P79" t="s">
+      <c r="R79" t="s">
         <v>304</v>
       </c>
-      <c r="Q79" t="s">
+      <c r="S79" t="s">
         <v>305</v>
       </c>
-      <c r="R79" t="s">
+      <c r="T79" t="s">
         <v>306</v>
-      </c>
-      <c r="S79" t="s">
-        <v>307</v>
-      </c>
-      <c r="T79" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="80" spans="2:20" x14ac:dyDescent="0.2">
@@ -7988,7 +8028,7 @@
         <v>148</v>
       </c>
       <c r="M80" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O80" t="s">
         <v>21</v>
@@ -8042,7 +8082,7 @@
         <v>148</v>
       </c>
       <c r="M81" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="O81" t="s">
         <v>21</v>
@@ -8096,7 +8136,7 @@
         <v>148</v>
       </c>
       <c r="M82" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="O82" t="s">
         <v>21</v>
@@ -8125,7 +8165,7 @@
         <v>255</v>
       </c>
       <c r="D83" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E83" t="s">
         <v>143</v>
@@ -8152,7 +8192,7 @@
         <v>280</v>
       </c>
       <c r="M83" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="N83">
         <v>2</v>
@@ -8178,10 +8218,10 @@
     </row>
     <row r="84" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D84" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E84" t="s">
         <v>143</v>
@@ -8208,7 +8248,7 @@
         <v>280</v>
       </c>
       <c r="M84" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="N84">
         <v>3</v>
@@ -8234,10 +8274,10 @@
     </row>
     <row r="85" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D85" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E85" t="s">
         <v>282</v>
@@ -8264,7 +8304,7 @@
         <v>280</v>
       </c>
       <c r="M85" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="N85">
         <v>3</v>
@@ -8290,10 +8330,10 @@
     </row>
     <row r="86" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B86" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D86" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E86" t="s">
         <v>143</v>
@@ -8320,7 +8360,7 @@
         <v>280</v>
       </c>
       <c r="M86" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="O86" t="s">
         <v>21</v>
@@ -8370,7 +8410,7 @@
         <v>148</v>
       </c>
       <c r="M87" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O87" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
updated seropositivity data from Pernille, attempted to fix data matrix to run adonis.
</commit_message>
<xml_diff>
--- a/metadata_unified.xlsx
+++ b/metadata_unified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elsa/Desktop/THESIS/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D2167A-ED5D-6E45-B0FB-790FE3E6D591}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101F5D1C-0109-0D47-9399-AE12AD68B910}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22660" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="500" windowWidth="22660" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="329">
   <si>
     <t>sample</t>
   </si>
@@ -1004,6 +1004,9 @@
   </si>
   <si>
     <t>sero_trichincella_spp</t>
+  </si>
+  <si>
+    <t>DUPLICATE</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1086,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1091,11 +1094,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1116,6 +1156,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1457,7 +1510,7 @@
   <dimension ref="A1:AE87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N56" sqref="N56"/>
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1602,11 +1655,11 @@
       <c r="J2" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>280</v>
+      <c r="K2" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="M2" t="s">
         <v>313</v>
@@ -1786,11 +1839,11 @@
       <c r="J4" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="K4" s="9" t="s">
-        <v>280</v>
+      <c r="K4" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M4" t="s">
         <v>313</v>
@@ -1967,11 +2020,11 @@
       <c r="J6" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>281</v>
+      <c r="K6" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="M6" t="s">
         <v>316</v>
@@ -2062,11 +2115,11 @@
       <c r="J7" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="K7" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>281</v>
+      <c r="K7" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>317</v>
@@ -2157,11 +2210,11 @@
       <c r="J8" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K8" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>281</v>
+      <c r="K8" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>315</v>
@@ -2252,11 +2305,11 @@
       <c r="J9" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K9" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>281</v>
+      <c r="K9" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="M9" s="6" t="s">
         <v>318</v>
@@ -2345,11 +2398,11 @@
       <c r="J10" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K10" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>280</v>
+      <c r="K10" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>314</v>
@@ -2436,11 +2489,11 @@
       <c r="J11" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K11" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>280</v>
+      <c r="K11" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>311</v>
@@ -2527,11 +2580,11 @@
       <c r="J12" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K12" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>280</v>
+      <c r="K12" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>309</v>
@@ -2596,34 +2649,34 @@
       <c r="B13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="19" t="s">
         <v>288</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="F13" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="L13" s="10" t="s">
+      <c r="F13" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="L13" s="22" t="s">
         <v>281</v>
       </c>
       <c r="M13" s="5" t="s">
@@ -2714,10 +2767,10 @@
         <v>280</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>314</v>
@@ -2806,8 +2859,8 @@
       <c r="J15" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K15" s="11" t="s">
-        <v>280</v>
+      <c r="K15" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="L15" s="13" t="s">
         <v>148</v>
@@ -2901,11 +2954,11 @@
       <c r="J16" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K16" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="L16" s="12" t="s">
-        <v>281</v>
+      <c r="K16" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M16" s="5" t="s">
         <v>319</v>
@@ -2996,11 +3049,11 @@
       <c r="J17" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="K17" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>281</v>
+      <c r="K17" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>318</v>
@@ -3091,11 +3144,11 @@
       <c r="J18" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K18" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>281</v>
+      <c r="K18" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>320</v>
@@ -3186,11 +3239,11 @@
       <c r="J19" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K19" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="L19" s="12" t="s">
-        <v>281</v>
+      <c r="K19" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M19" s="5" t="s">
         <v>321</v>
@@ -3348,35 +3401,35 @@
       <c r="B21" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="J21" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>281</v>
+      <c r="F21" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="I21" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="J21" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M21" s="5" t="s">
         <v>322</v>
@@ -3466,10 +3519,10 @@
         <v>280</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L22" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M22" s="6" t="s">
         <v>309</v>
@@ -3534,34 +3587,34 @@
       <c r="B23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="19" t="s">
         <v>289</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="F23" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="L23" s="10" t="s">
+      <c r="F23" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="K23" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="L23" s="22" t="s">
         <v>281</v>
       </c>
       <c r="M23" s="5" t="s">
@@ -3653,11 +3706,11 @@
       <c r="J24" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K24" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="L24" s="12" t="s">
-        <v>281</v>
+      <c r="K24" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M24" s="6" t="s">
         <v>320</v>
@@ -3746,10 +3799,10 @@
         <v>280</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M25" s="6" t="s">
         <v>308</v>
@@ -3836,10 +3889,10 @@
         <v>280</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M26" s="6" t="s">
         <v>311</v>
@@ -3926,10 +3979,10 @@
         <v>280</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L27" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>313</v>
@@ -4015,10 +4068,10 @@
       <c r="J28" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="K28" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="L28" s="8" t="s">
+      <c r="K28" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L28" s="13" t="s">
         <v>148</v>
       </c>
       <c r="M28" s="6" t="s">
@@ -4108,11 +4161,11 @@
       <c r="J29" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K29" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="L29" s="12" t="s">
-        <v>281</v>
+      <c r="K29" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M29" s="6" t="s">
         <v>315</v>
@@ -4298,11 +4351,11 @@
       <c r="J31" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K31" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="L31" s="12" t="s">
-        <v>281</v>
+      <c r="K31" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M31" s="6" t="s">
         <v>318</v>
@@ -4391,10 +4444,10 @@
         <v>280</v>
       </c>
       <c r="K32" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L32" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M32" s="6" t="s">
         <v>313</v>
@@ -4481,10 +4534,10 @@
         <v>280</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L33" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M33" s="6" t="s">
         <v>307</v>
@@ -4549,35 +4602,35 @@
       <c r="B34" t="s">
         <v>93</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="F34" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="J34" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="K34" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="L34" s="13" t="s">
-        <v>148</v>
+      <c r="F34" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="H34" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="I34" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="J34" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="K34" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="L34" s="26" t="s">
+        <v>281</v>
       </c>
       <c r="M34" s="6" t="s">
         <v>319</v>
@@ -4666,10 +4719,10 @@
         <v>281</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L35" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M35" s="6" t="s">
         <v>313</v>
@@ -4756,10 +4809,10 @@
         <v>281</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L36" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M36" s="6" t="s">
         <v>307</v>
@@ -4846,10 +4899,10 @@
         <v>280</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L37" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M37" s="6" t="s">
         <v>314</v>
@@ -4938,11 +4991,11 @@
       <c r="J38" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K38" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="L38" s="12" t="s">
-        <v>281</v>
+      <c r="K38" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L38" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M38" s="6" t="s">
         <v>319</v>
@@ -5031,10 +5084,10 @@
         <v>280</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L39" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M39" s="6" t="s">
         <v>308</v>
@@ -5123,11 +5176,11 @@
       <c r="J40" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K40" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="L40" s="12" t="s">
-        <v>281</v>
+      <c r="K40" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L40" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M40" s="6" t="s">
         <v>315</v>
@@ -5311,10 +5364,10 @@
         <v>280</v>
       </c>
       <c r="K42" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L42" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>311</v>
@@ -5403,10 +5456,10 @@
       <c r="J43" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K43" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="L43" s="12" t="s">
+      <c r="K43" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L43" s="13" t="s">
         <v>148</v>
       </c>
       <c r="M43" s="6" t="s">
@@ -5496,10 +5549,10 @@
         <v>280</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M44" s="6" t="s">
         <v>311</v>
@@ -5564,35 +5617,35 @@
       <c r="B45" t="s">
         <v>115</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="F45" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="I45" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="J45" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="K45" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="L45" s="13" t="s">
-        <v>148</v>
+      <c r="F45" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="G45" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="H45" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="I45" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="J45" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="K45" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="L45" s="26" t="s">
+        <v>281</v>
       </c>
       <c r="M45" s="6" t="s">
         <v>319</v>
@@ -5683,11 +5736,11 @@
       <c r="J46" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K46" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="L46" s="12" t="s">
-        <v>281</v>
+      <c r="K46" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L46" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M46" s="6" t="s">
         <v>320</v>
@@ -5774,10 +5827,10 @@
         <v>280</v>
       </c>
       <c r="K47" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L47" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M47" s="6" t="s">
         <v>307</v>
@@ -5864,10 +5917,10 @@
         <v>280</v>
       </c>
       <c r="K48" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L48" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M48" s="6" t="s">
         <v>314</v>
@@ -5932,34 +5985,34 @@
       <c r="B49" t="s">
         <v>123</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="E49" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="F49" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="I49" s="12" t="s">
+      <c r="F49" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="H49" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="I49" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="J49" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="K49" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="L49" s="12" t="s">
+      <c r="J49" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="K49" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="L49" s="26" t="s">
         <v>281</v>
       </c>
       <c r="M49" s="6" t="s">
@@ -6049,10 +6102,10 @@
         <v>280</v>
       </c>
       <c r="K50" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L50" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M50" s="6" t="s">
         <v>314</v>
@@ -6139,10 +6192,10 @@
         <v>280</v>
       </c>
       <c r="K51" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L51" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M51" s="6" t="s">
         <v>309</v>
@@ -6231,11 +6284,11 @@
       <c r="J52" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="K52" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="L52" s="10" t="s">
-        <v>281</v>
+      <c r="K52" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L52" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M52" t="s">
         <v>324</v>
@@ -6326,11 +6379,11 @@
       <c r="J53" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K53" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="L53" s="12" t="s">
-        <v>281</v>
+      <c r="K53" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L53" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M53" s="6" t="s">
         <v>315</v>
@@ -6419,10 +6472,10 @@
         <v>280</v>
       </c>
       <c r="K54" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L54" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M54" s="6" t="s">
         <v>311</v>
@@ -6511,11 +6564,11 @@
       <c r="J55" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="K55" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="L55" s="12" t="s">
-        <v>281</v>
+      <c r="K55" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L55" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M55" s="6" t="s">
         <v>318</v>
@@ -6604,10 +6657,10 @@
         <v>280</v>
       </c>
       <c r="K56" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L56" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M56" s="6" t="s">
         <v>309</v>
@@ -6694,10 +6747,10 @@
         <v>280</v>
       </c>
       <c r="K57" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L57" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M57" s="6" t="s">
         <v>307</v>
@@ -6784,10 +6837,10 @@
         <v>280</v>
       </c>
       <c r="K58" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="L58" s="13" t="s">
-        <v>280</v>
+        <v>148</v>
       </c>
       <c r="M58" s="6" t="s">
         <v>311</v>
@@ -6876,11 +6929,11 @@
       <c r="J59" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="K59" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="L59" s="10" t="s">
-        <v>281</v>
+      <c r="K59" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L59" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="M59" t="s">
         <v>323</v>
@@ -7152,7 +7205,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>151</v>
       </c>
@@ -7205,7 +7258,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>152</v>
       </c>
@@ -7258,7 +7311,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>153</v>
       </c>
@@ -7311,7 +7364,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>154</v>
       </c>
@@ -7364,7 +7417,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>155</v>
       </c>
@@ -7417,7 +7470,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>156</v>
       </c>
@@ -7470,7 +7523,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>157</v>
       </c>
@@ -7523,7 +7576,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B72" s="2" t="s">
         <v>158</v>
       </c>
@@ -7582,7 +7635,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B73" s="2" t="s">
         <v>167</v>
       </c>
@@ -7641,7 +7694,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B74" s="2" t="s">
         <v>169</v>
       </c>
@@ -7700,7 +7753,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B75" s="2" t="s">
         <v>171</v>
       </c>
@@ -7759,7 +7812,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B76" s="2" t="s">
         <v>173</v>
       </c>
@@ -7818,7 +7871,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B77" s="2" t="s">
         <v>181</v>
       </c>
@@ -7877,7 +7930,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B78" s="2" t="s">
         <v>184</v>
       </c>
@@ -7936,7 +7989,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>328</v>
+      </c>
       <c r="B79" s="2" t="s">
         <v>191</v>
       </c>
@@ -7995,7 +8051,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="80" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B80" s="4" t="s">
         <v>204</v>
       </c>

</xml_diff>